<commit_message>
Add additional apps and interop
</commit_message>
<xml_diff>
--- a/how-to/integrate-with-excel/public/assets/excel-interop-example.xlsx
+++ b/how-to/integrate-with-excel/public/assets/excel-interop-example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workarea\openfin.co\workspace-starter\how-to\integrate-with-excel\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896CF292-1276-4212-8D57-9F9125F6689E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DA5456-B193-4F8E-BDAD-AF2CE3757272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6789" yWindow="2194" windowWidth="22397" windowHeight="13055" xr2:uid="{7E041702-BB2F-410C-9E81-E388169B1020}"/>
+    <workbookView xWindow="3763" yWindow="5829" windowWidth="25834" windowHeight="10542" xr2:uid="{7E041702-BB2F-410C-9E81-E388169B1020}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -78,37 +78,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF00CC88"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FF8C61FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFFF8C4C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
+        <fgColor rgb="FFFF5E60"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
+        <fgColor rgb="FFFF8FB8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor rgb="FFE9FF8F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -139,6 +139,17 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFE9FF8F"/>
+      <color rgb="FFFF8FB8"/>
+      <color rgb="FFFF5E60"/>
+      <color rgb="FFFF8C4C"/>
+      <color rgb="FF8C61FF"/>
+      <color rgb="FF00CC88"/>
+      <color rgb="FFFC9AFA"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>

</xml_diff>